<commit_message>
Added orchestration with Airflow
</commit_message>
<xml_diff>
--- a/data_source/pdowntime.xlsx
+++ b/data_source/pdowntime.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,11 +469,11 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -487,11 +487,11 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -559,11 +559,11 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -577,11 +577,11 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -613,11 +613,11 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -649,11 +649,11 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -685,11 +685,11 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -739,11 +739,11 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -811,11 +811,11 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -829,11 +829,11 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -883,11 +883,11 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -919,11 +919,11 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -955,11 +955,11 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -991,11 +991,11 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -1027,11 +1027,11 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -1063,11 +1063,11 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1099,11 +1099,11 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1315,11 +1315,11 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -1351,11 +1351,11 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -1549,11 +1549,11 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -1585,11 +1585,11 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1621,11 +1621,11 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1639,11 +1639,11 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1657,11 +1657,11 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -1693,11 +1693,11 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -1729,11 +1729,11 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1819,11 +1819,11 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1873,11 +1873,11 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -1927,11 +1927,11 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1963,11 +1963,11 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2089,11 +2089,11 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2179,11 +2179,11 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -2323,11 +2323,11 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2341,11 +2341,11 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2413,11 +2413,11 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -2431,11 +2431,11 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -2503,11 +2503,11 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -2521,11 +2521,11 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -2575,11 +2575,11 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -2683,11 +2683,11 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -2701,11 +2701,11 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2719,11 +2719,11 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -2737,11 +2737,11 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -2773,11 +2773,11 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -2795,7 +2795,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -2809,11 +2809,11 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2845,11 +2845,11 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3061,11 +3061,11 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -3241,11 +3241,11 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -3277,11 +3277,11 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -3331,11 +3331,11 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -3367,11 +3367,11 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -3403,11 +3403,11 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -3457,11 +3457,11 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3511,11 +3511,11 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -3547,11 +3547,11 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -3619,11 +3619,11 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -3727,11 +3727,11 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -3745,11 +3745,11 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -3871,11 +3871,11 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -3889,11 +3889,11 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3907,11 +3907,11 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3925,11 +3925,11 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -3979,11 +3979,11 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3997,11 +3997,11 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4015,11 +4015,11 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -4033,11 +4033,11 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4069,11 +4069,11 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4123,11 +4123,11 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -4141,11 +4141,11 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4177,11 +4177,11 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -4195,11 +4195,11 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -4375,11 +4375,11 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -4393,11 +4393,11 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -4501,11 +4501,11 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -4537,11 +4537,11 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4573,11 +4573,11 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -4627,11 +4627,11 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -4663,11 +4663,11 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4717,11 +4717,11 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -4753,11 +4753,11 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -4771,11 +4771,11 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4843,11 +4843,11 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -4897,11 +4897,11 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -4933,11 +4933,11 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4969,7 +4969,7 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D252" t="inlineStr">
         <is>
@@ -4987,11 +4987,11 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -5077,11 +5077,11 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -5167,11 +5167,11 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -5221,11 +5221,11 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -5383,11 +5383,11 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -5617,11 +5617,11 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -5653,11 +5653,11 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -5761,11 +5761,11 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -5815,11 +5815,11 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -5887,11 +5887,11 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -5905,11 +5905,11 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -5995,11 +5995,11 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -6031,11 +6031,11 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6067,11 +6067,11 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6139,11 +6139,11 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6157,11 +6157,11 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6211,11 +6211,11 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -6247,11 +6247,11 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -6265,11 +6265,11 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -6283,11 +6283,11 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -6373,11 +6373,11 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6391,11 +6391,11 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -6409,11 +6409,11 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -6427,11 +6427,11 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -6445,11 +6445,11 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6661,11 +6661,11 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -6733,11 +6733,11 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6751,11 +6751,11 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6769,11 +6769,11 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -6841,11 +6841,11 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -6859,11 +6859,11 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6877,11 +6877,11 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6931,11 +6931,11 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -7003,11 +7003,11 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7057,11 +7057,11 @@
         </is>
       </c>
       <c r="C368" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7093,11 +7093,11 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -7111,11 +7111,11 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7165,11 +7165,11 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7219,11 +7219,11 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -7255,11 +7255,11 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7291,11 +7291,11 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -7381,11 +7381,11 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7399,11 +7399,11 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7417,11 +7417,11 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D388" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7561,11 +7561,11 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -7597,11 +7597,11 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7615,11 +7615,11 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7651,7 +7651,7 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D401" t="inlineStr">
         <is>
@@ -7705,11 +7705,11 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -7777,11 +7777,11 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7993,11 +7993,11 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8047,11 +8047,11 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8065,11 +8065,11 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D424" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -8101,11 +8101,11 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -8191,11 +8191,11 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D431" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8245,11 +8245,11 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D434" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -8263,11 +8263,11 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D435" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -8299,11 +8299,11 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D437" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8317,11 +8317,11 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D438" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -8443,11 +8443,11 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D445" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -8551,11 +8551,11 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D451" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -8641,11 +8641,11 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D456" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -8677,11 +8677,11 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D458" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8695,11 +8695,11 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D459" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -8713,11 +8713,11 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D460" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -8893,11 +8893,11 @@
         </is>
       </c>
       <c r="C470" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D470" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -9041,7 +9041,7 @@
       </c>
       <c r="D478" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -9073,11 +9073,11 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -9109,11 +9109,11 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D482" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -9145,11 +9145,11 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D484" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -9181,11 +9181,11 @@
         </is>
       </c>
       <c r="C486" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D486" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9253,11 +9253,11 @@
         </is>
       </c>
       <c r="C490" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9271,11 +9271,11 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9379,11 +9379,11 @@
         </is>
       </c>
       <c r="C497" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D497" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9397,11 +9397,11 @@
         </is>
       </c>
       <c r="C498" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -9415,11 +9415,11 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D499" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9451,11 +9451,11 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D501" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9505,11 +9505,11 @@
         </is>
       </c>
       <c r="C504" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -9559,11 +9559,11 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D507" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9595,11 +9595,11 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -9631,11 +9631,11 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D511" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9667,11 +9667,11 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D513" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -9721,11 +9721,11 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D516" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9811,11 +9811,11 @@
         </is>
       </c>
       <c r="C521" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D521" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -9955,11 +9955,11 @@
         </is>
       </c>
       <c r="C529" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D529" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -10009,11 +10009,11 @@
         </is>
       </c>
       <c r="C532" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D532" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10027,11 +10027,11 @@
         </is>
       </c>
       <c r="C533" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D533" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -10099,11 +10099,11 @@
         </is>
       </c>
       <c r="C537" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D537" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10117,11 +10117,11 @@
         </is>
       </c>
       <c r="C538" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D538" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -10135,11 +10135,11 @@
         </is>
       </c>
       <c r="C539" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D539" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -10153,11 +10153,11 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D540" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -10225,11 +10225,11 @@
         </is>
       </c>
       <c r="C544" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D544" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -10279,11 +10279,11 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D547" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -10315,11 +10315,11 @@
         </is>
       </c>
       <c r="C549" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D549" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10351,11 +10351,11 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D551" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -10459,11 +10459,11 @@
         </is>
       </c>
       <c r="C557" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D557" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10495,11 +10495,11 @@
         </is>
       </c>
       <c r="C559" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D559" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -10657,11 +10657,11 @@
         </is>
       </c>
       <c r="C568" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D568" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10675,11 +10675,11 @@
         </is>
       </c>
       <c r="C569" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D569" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10693,11 +10693,11 @@
         </is>
       </c>
       <c r="C570" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D570" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -10801,11 +10801,11 @@
         </is>
       </c>
       <c r="C576" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D576" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -10855,11 +10855,11 @@
         </is>
       </c>
       <c r="C579" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D579" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10945,11 +10945,11 @@
         </is>
       </c>
       <c r="C584" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D584" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -10963,11 +10963,11 @@
         </is>
       </c>
       <c r="C585" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D585" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -11053,11 +11053,11 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D590" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -11089,11 +11089,11 @@
         </is>
       </c>
       <c r="C592" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D592" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -11107,11 +11107,11 @@
         </is>
       </c>
       <c r="C593" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D593" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11161,11 +11161,11 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D596" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -11251,11 +11251,11 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D601" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -11287,7 +11287,7 @@
         </is>
       </c>
       <c r="C603" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D603" t="inlineStr">
         <is>
@@ -11323,11 +11323,11 @@
         </is>
       </c>
       <c r="C605" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D605" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -11341,11 +11341,11 @@
         </is>
       </c>
       <c r="C606" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D606" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11395,11 +11395,11 @@
         </is>
       </c>
       <c r="C609" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D609" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -11431,11 +11431,11 @@
         </is>
       </c>
       <c r="C611" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -11503,11 +11503,11 @@
         </is>
       </c>
       <c r="C615" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D615" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11539,11 +11539,11 @@
         </is>
       </c>
       <c r="C617" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D617" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11557,11 +11557,11 @@
         </is>
       </c>
       <c r="C618" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D618" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11575,11 +11575,11 @@
         </is>
       </c>
       <c r="C619" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D619" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11593,11 +11593,11 @@
         </is>
       </c>
       <c r="C620" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D620" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11611,11 +11611,11 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D621" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -11647,11 +11647,11 @@
         </is>
       </c>
       <c r="C623" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D623" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11683,11 +11683,11 @@
         </is>
       </c>
       <c r="C625" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D625" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11719,11 +11719,11 @@
         </is>
       </c>
       <c r="C627" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D627" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -11737,11 +11737,11 @@
         </is>
       </c>
       <c r="C628" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D628" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11755,11 +11755,11 @@
         </is>
       </c>
       <c r="C629" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D629" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11791,11 +11791,11 @@
         </is>
       </c>
       <c r="C631" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D631" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11917,11 +11917,11 @@
         </is>
       </c>
       <c r="C638" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D638" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -11935,11 +11935,11 @@
         </is>
       </c>
       <c r="C639" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D639" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11989,11 +11989,11 @@
         </is>
       </c>
       <c r="C642" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D642" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12043,11 +12043,11 @@
         </is>
       </c>
       <c r="C645" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D645" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12061,11 +12061,11 @@
         </is>
       </c>
       <c r="C646" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D646" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -12097,11 +12097,11 @@
         </is>
       </c>
       <c r="C648" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D648" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12241,11 +12241,11 @@
         </is>
       </c>
       <c r="C656" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D656" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -12331,11 +12331,11 @@
         </is>
       </c>
       <c r="C661" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D661" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12367,11 +12367,11 @@
         </is>
       </c>
       <c r="C663" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D663" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -12385,11 +12385,11 @@
         </is>
       </c>
       <c r="C664" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D664" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12457,11 +12457,11 @@
         </is>
       </c>
       <c r="C668" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D668" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -12583,11 +12583,11 @@
         </is>
       </c>
       <c r="C675" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D675" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -12619,11 +12619,11 @@
         </is>
       </c>
       <c r="C677" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D677" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12655,11 +12655,11 @@
         </is>
       </c>
       <c r="C679" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D679" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -12673,11 +12673,11 @@
         </is>
       </c>
       <c r="C680" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D680" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12691,11 +12691,11 @@
         </is>
       </c>
       <c r="C681" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D681" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -12799,11 +12799,11 @@
         </is>
       </c>
       <c r="C687" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D687" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -12817,11 +12817,11 @@
         </is>
       </c>
       <c r="C688" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D688" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12835,11 +12835,11 @@
         </is>
       </c>
       <c r="C689" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D689" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12925,11 +12925,11 @@
         </is>
       </c>
       <c r="C694" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D694" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -12943,11 +12943,11 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D695" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -12961,11 +12961,11 @@
         </is>
       </c>
       <c r="C696" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D696" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -13051,11 +13051,11 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D701" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -13091,7 +13091,7 @@
       </c>
       <c r="D703" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -13123,11 +13123,11 @@
         </is>
       </c>
       <c r="C705" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D705" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -13141,11 +13141,11 @@
         </is>
       </c>
       <c r="C706" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D706" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -13213,11 +13213,11 @@
         </is>
       </c>
       <c r="C710" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D710" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -13267,11 +13267,11 @@
         </is>
       </c>
       <c r="C713" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D713" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -13285,11 +13285,11 @@
         </is>
       </c>
       <c r="C714" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D714" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -13339,11 +13339,11 @@
         </is>
       </c>
       <c r="C717" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D717" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13357,11 +13357,11 @@
         </is>
       </c>
       <c r="C718" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D718" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -13393,11 +13393,11 @@
         </is>
       </c>
       <c r="C720" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D720" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13411,11 +13411,11 @@
         </is>
       </c>
       <c r="C721" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D721" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -13447,11 +13447,11 @@
         </is>
       </c>
       <c r="C723" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D723" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -13501,11 +13501,11 @@
         </is>
       </c>
       <c r="C726" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D726" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -13537,11 +13537,11 @@
         </is>
       </c>
       <c r="C728" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D728" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13573,11 +13573,11 @@
         </is>
       </c>
       <c r="C730" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D730" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13609,11 +13609,11 @@
         </is>
       </c>
       <c r="C732" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D732" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -13627,11 +13627,11 @@
         </is>
       </c>
       <c r="C733" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D733" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Created the Dockerfile to install the dependencies in the containers, by creating a new image
</commit_message>
<xml_diff>
--- a/data_source/pdowntime.xlsx
+++ b/data_source/pdowntime.xlsx
@@ -469,11 +469,11 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -559,11 +559,11 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -613,11 +613,11 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -685,11 +685,11 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -721,11 +721,11 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -757,11 +757,11 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -793,11 +793,11 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -883,11 +883,11 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -901,11 +901,11 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -919,11 +919,11 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -955,11 +955,11 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -973,11 +973,11 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -991,11 +991,11 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1027,11 +1027,11 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1315,7 +1315,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1351,11 +1351,11 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1459,11 +1459,11 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -1549,11 +1549,11 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -1657,11 +1657,11 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1693,11 +1693,11 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -1873,11 +1873,11 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2035,11 +2035,11 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2179,11 +2179,11 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2287,11 +2287,11 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -2413,11 +2413,11 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2431,11 +2431,11 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2467,11 +2467,11 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -2503,11 +2503,11 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -2521,11 +2521,11 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2575,11 +2575,11 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2647,11 +2647,11 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -2683,11 +2683,11 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2701,11 +2701,11 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -2719,11 +2719,11 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2737,11 +2737,11 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2773,11 +2773,11 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2791,11 +2791,11 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -2881,11 +2881,11 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -2899,11 +2899,11 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -2953,11 +2953,11 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -2989,11 +2989,11 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -3061,11 +3061,11 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3241,11 +3241,11 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3259,11 +3259,11 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -3277,11 +3277,11 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3331,11 +3331,11 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3367,11 +3367,11 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3403,11 +3403,11 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3511,11 +3511,11 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3547,11 +3547,11 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -3601,11 +3601,11 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3619,11 +3619,11 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3727,11 +3727,11 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -3745,11 +3745,11 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3871,11 +3871,11 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3925,11 +3925,11 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -3961,11 +3961,11 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4015,11 +4015,11 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -4123,11 +4123,11 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4177,11 +4177,11 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4195,11 +4195,11 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4213,11 +4213,11 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -4285,11 +4285,11 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -4357,11 +4357,11 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -4375,11 +4375,11 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4393,11 +4393,11 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4429,11 +4429,11 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -4501,11 +4501,11 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4519,11 +4519,11 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -4573,11 +4573,11 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4627,11 +4627,11 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4717,11 +4717,11 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4753,11 +4753,11 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4825,11 +4825,11 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -4843,11 +4843,11 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4897,11 +4897,11 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -4969,7 +4969,7 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D252" t="inlineStr">
         <is>
@@ -5023,11 +5023,11 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -5077,11 +5077,11 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -5113,11 +5113,11 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -5257,11 +5257,11 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -5311,11 +5311,11 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -5383,11 +5383,11 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -5437,11 +5437,11 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -5455,11 +5455,11 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -5617,11 +5617,11 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -5653,11 +5653,11 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -5725,11 +5725,11 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -5815,11 +5815,11 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -5905,11 +5905,11 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -5995,7 +5995,7 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D309" t="inlineStr">
         <is>
@@ -6013,11 +6013,11 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -6049,11 +6049,11 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -6139,11 +6139,11 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -6211,11 +6211,11 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6247,11 +6247,11 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6265,11 +6265,11 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6283,11 +6283,11 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6301,11 +6301,11 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -6355,11 +6355,11 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -6391,11 +6391,11 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6409,11 +6409,11 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6427,11 +6427,11 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6481,11 +6481,11 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -6553,11 +6553,11 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -6661,11 +6661,11 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6769,11 +6769,11 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -6841,11 +6841,11 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -6859,11 +6859,11 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -6913,11 +6913,11 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -6935,7 +6935,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -6949,11 +6949,11 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -7003,11 +7003,11 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -7093,11 +7093,11 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7219,11 +7219,11 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7291,11 +7291,11 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7309,11 +7309,11 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -7345,11 +7345,11 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -7561,11 +7561,11 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -7615,11 +7615,11 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -7633,11 +7633,11 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D400" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -7651,11 +7651,11 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -7705,11 +7705,11 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8065,11 +8065,11 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D424" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -8101,11 +8101,11 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8137,11 +8137,11 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D428" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -8245,11 +8245,11 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D434" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8263,11 +8263,11 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D435" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8299,11 +8299,11 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D437" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -8317,11 +8317,11 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D438" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8335,11 +8335,11 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D439" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -8425,11 +8425,11 @@
         </is>
       </c>
       <c r="C444" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -8443,11 +8443,11 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D445" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8479,11 +8479,11 @@
         </is>
       </c>
       <c r="C447" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D447" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -8497,11 +8497,11 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D448" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -8551,11 +8551,11 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D451" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8587,11 +8587,11 @@
         </is>
       </c>
       <c r="C453" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D453" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -8623,11 +8623,11 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D455" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Power Outage</t>
         </is>
       </c>
     </row>
@@ -8641,11 +8641,11 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D456" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8659,11 +8659,11 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D457" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -8695,11 +8695,11 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D459" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8713,11 +8713,11 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D460" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -8749,11 +8749,11 @@
         </is>
       </c>
       <c r="C462" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D462" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -8803,11 +8803,11 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -8893,11 +8893,11 @@
         </is>
       </c>
       <c r="C470" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D470" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9037,11 +9037,11 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D478" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9073,11 +9073,11 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9109,11 +9109,11 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D482" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9145,7 +9145,7 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D484" t="inlineStr">
         <is>
@@ -9217,11 +9217,11 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -9235,11 +9235,11 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D489" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -9271,11 +9271,11 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -9397,11 +9397,11 @@
         </is>
       </c>
       <c r="C498" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9415,11 +9415,11 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D499" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -9469,11 +9469,11 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -9505,11 +9505,11 @@
         </is>
       </c>
       <c r="C504" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9599,7 +9599,7 @@
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -9667,11 +9667,11 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D513" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -9811,11 +9811,11 @@
         </is>
       </c>
       <c r="C521" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D521" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -9829,11 +9829,11 @@
         </is>
       </c>
       <c r="C522" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D522" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -9937,11 +9937,11 @@
         </is>
       </c>
       <c r="C528" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D528" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -9955,11 +9955,11 @@
         </is>
       </c>
       <c r="C529" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D529" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10027,11 +10027,11 @@
         </is>
       </c>
       <c r="C533" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D533" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10117,11 +10117,11 @@
         </is>
       </c>
       <c r="C538" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D538" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10135,11 +10135,11 @@
         </is>
       </c>
       <c r="C539" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D539" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10153,11 +10153,11 @@
         </is>
       </c>
       <c r="C540" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D540" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -10225,11 +10225,11 @@
         </is>
       </c>
       <c r="C544" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D544" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10279,11 +10279,11 @@
         </is>
       </c>
       <c r="C547" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D547" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10351,11 +10351,11 @@
         </is>
       </c>
       <c r="C551" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D551" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10405,11 +10405,11 @@
         </is>
       </c>
       <c r="C554" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D554" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -10477,11 +10477,11 @@
         </is>
       </c>
       <c r="C558" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D558" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -10495,11 +10495,11 @@
         </is>
       </c>
       <c r="C559" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D559" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -10621,11 +10621,11 @@
         </is>
       </c>
       <c r="C566" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D566" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -10693,11 +10693,11 @@
         </is>
       </c>
       <c r="C570" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D570" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10711,11 +10711,11 @@
         </is>
       </c>
       <c r="C571" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D571" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -10729,11 +10729,11 @@
         </is>
       </c>
       <c r="C572" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D572" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -10801,11 +10801,11 @@
         </is>
       </c>
       <c r="C576" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D576" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10945,11 +10945,11 @@
         </is>
       </c>
       <c r="C584" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D584" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -10963,11 +10963,11 @@
         </is>
       </c>
       <c r="C585" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D585" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11053,7 +11053,7 @@
         </is>
       </c>
       <c r="C590" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D590" t="inlineStr">
         <is>
@@ -11071,11 +11071,11 @@
         </is>
       </c>
       <c r="C591" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D591" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -11089,11 +11089,11 @@
         </is>
       </c>
       <c r="C592" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D592" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11125,11 +11125,11 @@
         </is>
       </c>
       <c r="C594" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D594" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -11143,11 +11143,11 @@
         </is>
       </c>
       <c r="C595" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D595" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -11161,11 +11161,11 @@
         </is>
       </c>
       <c r="C596" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D596" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11233,11 +11233,11 @@
         </is>
       </c>
       <c r="C600" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D600" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -11251,11 +11251,11 @@
         </is>
       </c>
       <c r="C601" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D601" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11269,11 +11269,11 @@
         </is>
       </c>
       <c r="C602" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D602" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -11287,11 +11287,11 @@
         </is>
       </c>
       <c r="C603" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D603" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11323,11 +11323,11 @@
         </is>
       </c>
       <c r="C605" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D605" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11395,11 +11395,11 @@
         </is>
       </c>
       <c r="C609" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D609" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11431,11 +11431,11 @@
         </is>
       </c>
       <c r="C611" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -11485,11 +11485,11 @@
         </is>
       </c>
       <c r="C614" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D614" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -11611,11 +11611,11 @@
         </is>
       </c>
       <c r="C621" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D621" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11719,11 +11719,11 @@
         </is>
       </c>
       <c r="C627" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D627" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -11773,11 +11773,11 @@
         </is>
       </c>
       <c r="C630" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D630" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -11809,11 +11809,11 @@
         </is>
       </c>
       <c r="C632" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D632" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -11863,11 +11863,11 @@
         </is>
       </c>
       <c r="C635" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D635" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -11921,7 +11921,7 @@
       </c>
       <c r="D638" t="inlineStr">
         <is>
-          <t>Power Outage</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -11935,11 +11935,11 @@
         </is>
       </c>
       <c r="C639" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D639" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -11971,11 +11971,11 @@
         </is>
       </c>
       <c r="C641" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D641" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -12025,11 +12025,11 @@
         </is>
       </c>
       <c r="C644" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D644" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -12061,11 +12061,11 @@
         </is>
       </c>
       <c r="C646" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D646" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12097,11 +12097,11 @@
         </is>
       </c>
       <c r="C648" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D648" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -12241,11 +12241,11 @@
         </is>
       </c>
       <c r="C656" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D656" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12349,11 +12349,11 @@
         </is>
       </c>
       <c r="C662" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D662" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -12367,11 +12367,11 @@
         </is>
       </c>
       <c r="C663" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D663" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12457,11 +12457,11 @@
         </is>
       </c>
       <c r="C668" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D668" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12547,11 +12547,11 @@
         </is>
       </c>
       <c r="C673" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D673" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -12583,11 +12583,11 @@
         </is>
       </c>
       <c r="C675" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D675" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12619,11 +12619,11 @@
         </is>
       </c>
       <c r="C677" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D677" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -12655,11 +12655,11 @@
         </is>
       </c>
       <c r="C679" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D679" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12691,11 +12691,11 @@
         </is>
       </c>
       <c r="C681" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D681" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12799,11 +12799,11 @@
         </is>
       </c>
       <c r="C687" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D687" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12907,11 +12907,11 @@
         </is>
       </c>
       <c r="C693" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D693" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Raw Material Shortage</t>
         </is>
       </c>
     </row>
@@ -12943,11 +12943,11 @@
         </is>
       </c>
       <c r="C695" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D695" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -12961,11 +12961,11 @@
         </is>
       </c>
       <c r="C696" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D696" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>Mechanical Failure</t>
         </is>
       </c>
     </row>
@@ -13033,11 +13033,11 @@
         </is>
       </c>
       <c r="C700" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D700" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -13051,11 +13051,11 @@
         </is>
       </c>
       <c r="C701" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D701" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13069,11 +13069,11 @@
         </is>
       </c>
       <c r="C702" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D702" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -13087,11 +13087,11 @@
         </is>
       </c>
       <c r="C703" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D703" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13123,7 +13123,7 @@
         </is>
       </c>
       <c r="C705" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D705" t="inlineStr">
         <is>
@@ -13141,11 +13141,11 @@
         </is>
       </c>
       <c r="C706" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D706" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13213,11 +13213,11 @@
         </is>
       </c>
       <c r="C710" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D710" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13267,11 +13267,11 @@
         </is>
       </c>
       <c r="C713" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D713" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13285,11 +13285,11 @@
         </is>
       </c>
       <c r="C714" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D714" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13303,11 +13303,11 @@
         </is>
       </c>
       <c r="C715" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D715" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -13357,11 +13357,11 @@
         </is>
       </c>
       <c r="C718" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D718" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13411,11 +13411,11 @@
         </is>
       </c>
       <c r="C721" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D721" t="inlineStr">
         <is>
-          <t>Raw Material Shortage</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13447,11 +13447,11 @@
         </is>
       </c>
       <c r="C723" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D723" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13505,7 +13505,7 @@
       </c>
       <c r="D726" t="inlineStr">
         <is>
-          <t>Mechanical Failure</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>
@@ -13609,11 +13609,11 @@
         </is>
       </c>
       <c r="C732" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D732" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>No Downtime</t>
         </is>
       </c>
     </row>
@@ -13627,11 +13627,11 @@
         </is>
       </c>
       <c r="C733" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D733" t="inlineStr">
         <is>
-          <t>No Downtime</t>
+          <t>Maintenance</t>
         </is>
       </c>
     </row>

</xml_diff>